<commit_message>
Plot Figs. 3-9 from the manuscript
Had to add calculate_B2() to output.py for Fig. 9.
</commit_message>
<xml_diff>
--- a/data/exports.xlsx
+++ b/data/exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Drive/ucsc/code/pyrite-dev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84CE6E5-281E-774F-918C-5F3330F4C05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BDD94A-05E8-D945-A71A-2B9F92E7A692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14500" activeTab="4" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
+    <workbookView xWindow="780" yWindow="1720" windowWidth="25600" windowHeight="14500" activeTab="9" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
   </bookViews>
   <sheets>
     <sheet name="POC" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,11 @@
     <sheet name="POC_fluxes_thorium" sheetId="6" r:id="rId3"/>
     <sheet name="POC_fluxes_traps" sheetId="7" r:id="rId4"/>
     <sheet name="hydrography" sheetId="8" r:id="rId5"/>
+    <sheet name="C91_remin_EP" sheetId="9" r:id="rId6"/>
+    <sheet name="C91_remin_SP" sheetId="10" r:id="rId7"/>
+    <sheet name="C91_agg_EP" sheetId="11" r:id="rId8"/>
+    <sheet name="C91_disagg_EP" sheetId="12" r:id="rId9"/>
+    <sheet name="C91_agg_SP" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
   <si>
     <t>depth</t>
   </si>
@@ -140,6 +145,12 @@
   </si>
   <si>
     <t>cp_sd</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -1634,6 +1645,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45A9B29-B335-4948-8011-5883DC8AEC00}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20.6437569139635</v>
+      </c>
+      <c r="B2">
+        <v>8.6868158055079525E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>62.801984084502031</v>
+      </c>
+      <c r="B3">
+        <v>4.7762631113937061E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>139.56749812653865</v>
+      </c>
+      <c r="B4">
+        <v>2.1107875105605165E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>251.46843664132999</v>
+      </c>
+      <c r="B5">
+        <v>5.3212801835320804E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>357.07097741141166</v>
+      </c>
+      <c r="B6">
+        <v>4.7185201309897966E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CED31C6-DEAB-CD40-9B03-17A7DE5EE234}">
   <dimension ref="A1:D55"/>
@@ -2640,7 +2714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FF0389-B4F8-164E-8EED-AFBAAC4496EA}">
   <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -23190,4 +23264,453 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80233AEE-6E35-F949-A834-FE78C9CB1055}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>8.6941766906638023</v>
+      </c>
+      <c r="B2">
+        <v>5.1887519166817504E-2</v>
+      </c>
+      <c r="C2">
+        <v>2.9125986245435491E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>29.481097211318598</v>
+      </c>
+      <c r="B3">
+        <v>0.17834573270788434</v>
+      </c>
+      <c r="C3">
+        <v>6.8928148649265705E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>49.601374203765836</v>
+      </c>
+      <c r="B4">
+        <v>0.22605604030502335</v>
+      </c>
+      <c r="C4">
+        <v>8.1151250059975241E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>70.318831766124504</v>
+      </c>
+      <c r="B5">
+        <v>7.1119385749428873E-2</v>
+      </c>
+      <c r="C5">
+        <v>8.5575249689813129E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>88.870679241798939</v>
+      </c>
+      <c r="B6">
+        <v>3.3423448317960035E-2</v>
+      </c>
+      <c r="C6">
+        <v>9.1710494602632822E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>124.448982868203</v>
+      </c>
+      <c r="B7">
+        <v>2.2647475997286403E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.3536242934517464E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>173.92529113098567</v>
+      </c>
+      <c r="B8">
+        <v>2.0748539495342864E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.3705286288751593E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>248.43897587581168</v>
+      </c>
+      <c r="B9">
+        <v>5.3214442093876468E-3</v>
+      </c>
+      <c r="C9">
+        <v>1.7032242987605303E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>348.453018365383</v>
+      </c>
+      <c r="B10">
+        <v>4.0374998668797962E-3</v>
+      </c>
+      <c r="C10">
+        <v>1.1249889809502148E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>448.5886013584643</v>
+      </c>
+      <c r="B11">
+        <v>3.8772012879111305E-3</v>
+      </c>
+      <c r="C11">
+        <v>1.0966606931140719E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F7BD2D-5020-8141-89FD-5D3546635FED}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>55.395941820793595</v>
+      </c>
+      <c r="B2">
+        <v>0.83824398073072504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>105.74160531513701</v>
+      </c>
+      <c r="B3">
+        <v>0.83245874935401099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>170.34027653079499</v>
+      </c>
+      <c r="B4">
+        <v>0.46769066324557002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>281.401508349793</v>
+      </c>
+      <c r="B5">
+        <v>0.37472409368756898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>372.36263242951998</v>
+      </c>
+      <c r="B6">
+        <v>0.29328958573844699</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D8E802-594D-4B44-9284-6F8EF3026E0F}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30.779538389514801</v>
+      </c>
+      <c r="B2">
+        <v>3.5755287602703148E-2</v>
+      </c>
+      <c r="C2">
+        <v>1.221480423608781E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>50.762696418322506</v>
+      </c>
+      <c r="B3">
+        <v>0.1098734521292085</v>
+      </c>
+      <c r="C3">
+        <v>3.2958757026330471E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>80.614549035601641</v>
+      </c>
+      <c r="B4">
+        <v>1.068051531072498E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.7898566320013798E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>102.56885520043403</v>
+      </c>
+      <c r="B5">
+        <v>3.6202608301058176E-3</v>
+      </c>
+      <c r="C5">
+        <v>3.1062432888301515E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>142.430575011093</v>
+      </c>
+      <c r="B6">
+        <v>3.803948274387791E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.5793402002255984E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>176.05738930109601</v>
+      </c>
+      <c r="B7">
+        <v>3.9076993577098051E-3</v>
+      </c>
+      <c r="C7">
+        <v>3.0635592644699316E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>251.52270281350849</v>
+      </c>
+      <c r="B8">
+        <v>4.1392541442019401E-4</v>
+      </c>
+      <c r="C8">
+        <v>1.7856649965841207E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>350.73599599748798</v>
+      </c>
+      <c r="B9">
+        <v>3.5079720625418454E-4</v>
+      </c>
+      <c r="C9">
+        <v>1.3063288250004547E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>450.50505050505001</v>
+      </c>
+      <c r="B10">
+        <v>6.6707678067171505E-4</v>
+      </c>
+      <c r="C10">
+        <v>2.2271893440450347E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3FC757-4300-2E4C-925A-2B3B2C61B71D}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>22.955958455804033</v>
+      </c>
+      <c r="B2">
+        <v>2.4408240687267084</v>
+      </c>
+      <c r="C2">
+        <v>3.7012003460636045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>38.222762603422154</v>
+      </c>
+      <c r="B3">
+        <v>11.456281560284584</v>
+      </c>
+      <c r="C3">
+        <v>8.4560050018796087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>62.754550107915001</v>
+      </c>
+      <c r="B4">
+        <v>1.8590986074670099</v>
+      </c>
+      <c r="C4">
+        <v>6.5176777925329912</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>83.918352966768268</v>
+      </c>
+      <c r="B5">
+        <v>0.53386519163042168</v>
+      </c>
+      <c r="C5">
+        <v>3.2424976953722529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>119.07436454643467</v>
+      </c>
+      <c r="B6">
+        <v>0.66434574338343932</v>
+      </c>
+      <c r="C6">
+        <v>1.3124088751715686</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>168.15568328868335</v>
+      </c>
+      <c r="B7">
+        <v>1.8549043729611017</v>
+      </c>
+      <c r="C7">
+        <v>2.9107070376216595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>246.970035778175</v>
+      </c>
+      <c r="B8">
+        <v>0.1593487686009375</v>
+      </c>
+      <c r="C8">
+        <v>0.71447524318632871</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>345.6563059033985</v>
+      </c>
+      <c r="B9">
+        <v>0.17596721536045501</v>
+      </c>
+      <c r="C9">
+        <v>0.5081411796086448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>447.11538461538402</v>
+      </c>
+      <c r="B10">
+        <v>0.21228684221461899</v>
+      </c>
+      <c r="C10">
+        <v>1.008215057785381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct Clegg91 StationP Bm1s estimates
</commit_message>
<xml_diff>
--- a/data/exports.xlsx
+++ b/data/exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Drive/ucsc/code/pyrite-dev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BDD94A-05E8-D945-A71A-2B9F92E7A692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4555D7DA-315D-D748-893E-F7A69680DDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1720" windowWidth="25600" windowHeight="14500" activeTab="9" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
+    <workbookView xWindow="780" yWindow="1720" windowWidth="25600" windowHeight="14500" activeTab="6" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
   </bookViews>
   <sheets>
     <sheet name="POC" sheetId="3" r:id="rId1"/>
@@ -1649,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45A9B29-B335-4948-8011-5883DC8AEC00}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
@@ -23406,8 +23406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F7BD2D-5020-8141-89FD-5D3546635FED}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23422,42 +23422,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>55.395941820793595</v>
+        <v>41.787439613526601</v>
       </c>
       <c r="B2">
-        <v>0.83824398073072504</v>
+        <v>8.1854673070690206E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>105.74160531513701</v>
+        <v>86.231884057970902</v>
       </c>
       <c r="B3">
-        <v>0.83245874935401099</v>
+        <v>8.1854673070690206E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>170.34027653079499</v>
+        <v>154.31763285024101</v>
       </c>
       <c r="B4">
-        <v>0.46769066324557002</v>
+        <v>4.5457829527820702E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>281.401508349793</v>
+        <v>265.94202898550702</v>
       </c>
       <c r="B5">
-        <v>0.37472409368756898</v>
+        <v>3.6746619407366801E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>372.36263242951998</v>
+        <v>366.54589371980597</v>
       </c>
       <c r="B6">
-        <v>0.29328958573844699</v>
+        <v>2.8610255691043699E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>